<commit_message>
change to trade Generic 1 Bonds futures
</commit_message>
<xml_diff>
--- a/Sigmaa005/Sigmaa005ScoreBoard.xlsx
+++ b/Sigmaa005/Sigmaa005ScoreBoard.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
   <si>
     <t>timestamp</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>T-model signal (combined)</t>
+  </si>
+  <si>
+    <t>DAX</t>
   </si>
 </sst>
 </file>
@@ -154,7 +157,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -498,20 +501,20 @@
     <xf numFmtId="14" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -523,17 +526,17 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1495,7 +1498,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
@@ -1503,9 +1506,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1537,22 +1540,22 @@
         <v>14</v>
       </c>
       <c r="B2" s="19">
-        <v>43077</v>
+        <v>43202</v>
       </c>
       <c r="C2">
-        <v>18.649979791668912</v>
+        <v>5.7402213506523632</v>
       </c>
       <c r="D2">
-        <v>-3.9663832799179333</v>
+        <v>-0.97341583846487134</v>
       </c>
       <c r="E2">
-        <v>20</v>
+        <v>1.9044519681442327</v>
       </c>
       <c r="F2">
-        <v>20</v>
+        <v>5.8118930175807035</v>
       </c>
       <c r="G2">
-        <v>20</v>
+        <v>7.5034108265953714</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1560,22 +1563,22 @@
         <v>15</v>
       </c>
       <c r="B3" s="19">
-        <v>43077</v>
+        <v>43202</v>
       </c>
       <c r="C3">
-        <v>20</v>
+        <v>9.1926037297326726</v>
       </c>
       <c r="D3">
-        <v>16.684601942494112</v>
+        <v>11.071906557705075</v>
       </c>
       <c r="E3">
-        <v>5.5733560361472074</v>
+        <v>-3.1249848846569099</v>
       </c>
       <c r="F3">
-        <v>9.4708503763952407</v>
+        <v>1.5561839012784087</v>
       </c>
       <c r="G3">
-        <v>13.169748687254344</v>
+        <v>7.1870144627716224</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1583,22 +1586,22 @@
         <v>16</v>
       </c>
       <c r="B4" s="19">
-        <v>43077</v>
+        <v>43202</v>
       </c>
       <c r="C4">
-        <v>14.117317103061398</v>
+        <v>11.893659167996583</v>
       </c>
       <c r="D4">
-        <v>6.1042047741794132</v>
+        <v>14.962751586945219</v>
       </c>
       <c r="E4">
-        <v>6.6760150432087526</v>
+        <v>-3.9864128256911044</v>
       </c>
       <c r="F4">
-        <v>12.939308190275911</v>
+        <v>0.71743931090858926</v>
       </c>
       <c r="G4">
-        <v>15.960748162828573</v>
+        <v>6.0273566265938756</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1606,22 +1609,22 @@
         <v>17</v>
       </c>
       <c r="B5" s="19">
-        <v>43077</v>
+        <v>43202</v>
       </c>
       <c r="C5">
-        <v>17.091866230778372</v>
+        <v>7.8894100441314787</v>
       </c>
       <c r="D5">
-        <v>13.712218946388495</v>
+        <v>9.0601177926637089</v>
       </c>
       <c r="E5">
-        <v>2.6779809153096328</v>
+        <v>6.5107556788116838</v>
       </c>
       <c r="F5">
-        <v>12.547723341745744</v>
+        <v>-1.648741041082459</v>
       </c>
       <c r="G5">
-        <v>17.252387856012099</v>
+        <v>-1.9900944311644155</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1629,22 +1632,22 @@
         <v>18</v>
       </c>
       <c r="B6" s="19">
-        <v>43077</v>
+        <v>43202</v>
       </c>
       <c r="C6">
-        <v>10.880619988235393</v>
+        <v>9.4318026430809532</v>
       </c>
       <c r="D6">
-        <v>-2.4731373805448338</v>
+        <v>8.6643598196580474</v>
       </c>
       <c r="E6">
-        <v>7.8701676278994714</v>
+        <v>-2.0895562836341606</v>
       </c>
       <c r="F6">
-        <v>15.348880010914966</v>
+        <v>4.7499633479461512</v>
       </c>
       <c r="G6">
-        <v>18.758352756514391</v>
+        <v>11.477478137787582</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1652,22 +1655,22 @@
         <v>19</v>
       </c>
       <c r="B7" s="19">
-        <v>43077</v>
+        <v>43203</v>
       </c>
       <c r="C7">
-        <v>-0.13176184313442998</v>
+        <v>0.44848005394504492</v>
       </c>
       <c r="D7">
-        <v>5.1543657242780014</v>
+        <v>7.9361794159837489</v>
       </c>
       <c r="E7">
-        <v>-7.8324374906191387</v>
+        <v>3.4445833664773353</v>
       </c>
       <c r="F7">
-        <v>-8.5947039734356263</v>
+        <v>-12.449710886312944</v>
       </c>
       <c r="G7">
-        <v>-8.4728924935434016</v>
+        <v>-15.318537170169225</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1675,22 +1678,22 @@
         <v>20</v>
       </c>
       <c r="B8" s="19">
-        <v>43077</v>
+        <v>43203</v>
       </c>
       <c r="C8">
-        <v>5.1251173626475781</v>
+        <v>6.2471313095442653</v>
       </c>
       <c r="D8">
-        <v>8.7804227669493464</v>
+        <v>10.761804814096337</v>
       </c>
       <c r="E8">
-        <v>0.87207028637587858</v>
+        <v>5.5490149701918474</v>
       </c>
       <c r="F8">
-        <v>-5.0987887349677736</v>
+        <v>-7.0063056639735963</v>
       </c>
       <c r="G8">
-        <v>-4.0304817883549955</v>
+        <v>-12.117767770460732</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1698,22 +1701,22 @@
         <v>21</v>
       </c>
       <c r="B9" s="19">
-        <v>43077</v>
+        <v>43203</v>
       </c>
       <c r="C9">
-        <v>4.5390661723477042</v>
+        <v>4.7637205081046554</v>
       </c>
       <c r="D9">
-        <v>2.6127257046025205</v>
+        <v>9.5274410162093108</v>
       </c>
       <c r="E9">
-        <v>4.8694807174907329</v>
+        <v>0</v>
       </c>
       <c r="F9">
-        <v>4.4203207053859659</v>
+        <v>0</v>
       </c>
       <c r="G9">
-        <v>1.9812018537549818</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1721,22 +1724,22 @@
         <v>22</v>
       </c>
       <c r="B10" s="19">
-        <v>43077</v>
+        <v>43203</v>
       </c>
       <c r="C10">
-        <v>16.466138844921783</v>
+        <v>15.690889177423504</v>
       </c>
       <c r="D10">
         <v>20</v>
       </c>
       <c r="E10">
-        <v>6.5112978406758648</v>
+        <v>10.617588522339645</v>
       </c>
       <c r="F10">
-        <v>1.9483452552699327</v>
+        <v>-4.5368558884230303</v>
       </c>
       <c r="G10">
-        <v>0.4445316178186407</v>
+        <v>-8.4037961491734166</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1744,22 +1747,22 @@
         <v>23</v>
       </c>
       <c r="B11" s="19">
-        <v>43077</v>
+        <v>43202</v>
       </c>
       <c r="C11">
-        <v>6.8468238631389529</v>
+        <v>8.6685046173644515</v>
       </c>
       <c r="D11">
-        <v>-1.1975654982263575</v>
+        <v>3.2817711759426516</v>
       </c>
       <c r="E11">
-        <v>8.4064333676840963</v>
+        <v>8.2752801270979859</v>
       </c>
       <c r="F11">
-        <v>17.299827711252725</v>
+        <v>9.4882856806693336</v>
       </c>
       <c r="G11">
-        <v>14.910973219370199</v>
+        <v>12.266451755101885</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1767,22 +1770,22 @@
         <v>24</v>
       </c>
       <c r="B12" s="19">
-        <v>43077</v>
+        <v>43203</v>
       </c>
       <c r="C12">
-        <v>-2.0548719693690178</v>
+        <v>-1.5573721835490968</v>
       </c>
       <c r="D12">
-        <v>-5.5443761439808892</v>
+        <v>-3.1147443670981936</v>
       </c>
       <c r="E12">
-        <v>-9.5228451661322939</v>
+        <v>0</v>
       </c>
       <c r="F12">
-        <v>-1.6439366871901808</v>
+        <v>0</v>
       </c>
       <c r="G12">
-        <v>3.9100686777555222</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1790,22 +1793,45 @@
         <v>25</v>
       </c>
       <c r="B13" s="19">
-        <v>43077</v>
+        <v>43203</v>
       </c>
       <c r="C13">
-        <v>-13.667537968539802</v>
+        <v>-16.559879116594324</v>
       </c>
       <c r="D13">
-        <v>-7.6659973982736611</v>
+        <v>-15.532888311392476</v>
       </c>
       <c r="E13">
-        <v>-14.510145679461202</v>
+        <v>4.5942347219017865</v>
       </c>
       <c r="F13">
-        <v>-7.9060284338763722</v>
+        <v>-15.811544175405892</v>
       </c>
       <c r="G13">
-        <v>-7.3680539041034327</v>
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>40</v>
+      </c>
+      <c r="B14" s="19">
+        <v>43202</v>
+      </c>
+      <c r="C14">
+        <v>-3.0558073289275525</v>
+      </c>
+      <c r="D14">
+        <v>0.14393696283560189</v>
+      </c>
+      <c r="E14">
+        <v>-4.5883094093854924</v>
+      </c>
+      <c r="F14">
+        <v>-6.6442603023127358</v>
+      </c>
+      <c r="G14">
+        <v>-0.80845670779221257</v>
       </c>
     </row>
   </sheetData>

</xml_diff>